<commit_message>
Changed Tank control to account for positive Level reading.  Need to figure our the Keyance sensor level scaling in case need to use differrent unit.
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00788a1fe100dfc/Documents/GitHub/PWC-OLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D2C35F2-EE84-41DD-B607-3C2E5EC3A0A9}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="680" windowWidth="15780" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="80" yWindow="1780" windowWidth="17180" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tank Calibrations" sheetId="1" r:id="rId1"/>
+    <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="LKe">'Tank Calibrations'!$D$2</definedName>
-    <definedName name="LKf">'Tank Calibrations'!$D$3</definedName>
-    <definedName name="LMe">'Tank Calibrations'!$E$2</definedName>
-    <definedName name="LMf">'Tank Calibrations'!$E$3</definedName>
-    <definedName name="LSe">'Tank Calibrations'!$C$2</definedName>
-    <definedName name="LSf">'Tank Calibrations'!$C$3</definedName>
+    <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
+    <definedName name="LKf">'Level Calibrations'!$D$3</definedName>
+    <definedName name="LMe">'Level Calibrations'!$E$2</definedName>
+    <definedName name="LMf">'Level Calibrations'!$E$3</definedName>
+    <definedName name="LSe">'Level Calibrations'!$C$2</definedName>
+    <definedName name="LSf">'Level Calibrations'!$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>M</t>
   </si>
@@ -116,12 +116,27 @@
   </si>
   <si>
     <t>LK (key raw)</t>
+  </si>
+  <si>
+    <t>Lse</t>
+  </si>
+  <si>
+    <t>Key Measure</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Full</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,12 +172,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -428,7 +446,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Mc = (LMf -LMe) /  (LKf -LKe)</a:t>
+            <a:t>Mc = (LMf -LMe) /  (LSf -LSe)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -940,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3BA94E-7FD5-4678-9436-02C8EAFB1FBB}">
-  <dimension ref="B1:J16"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -968,13 +986,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="D2" s="2">
-        <v>8.1999999999999993</v>
+        <v>1.1195999999999999</v>
       </c>
       <c r="E2" s="2">
-        <v>8.1999999999999993</v>
+        <v>8.4</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -991,13 +1009,13 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>8.5</v>
+        <v>1.956</v>
       </c>
       <c r="D3" s="2">
-        <v>2.5</v>
+        <v>7.6657999999999999</v>
       </c>
       <c r="E3" s="2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -1018,7 +1036,7 @@
       </c>
       <c r="D5" s="1">
         <f>(C3-C2)/(D3-D2)</f>
-        <v>-1.4912280701754388</v>
+        <v>-0.99966392716385089</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
@@ -1027,7 +1045,7 @@
       </c>
       <c r="D6" s="1">
         <f>C2-D5*D2</f>
-        <v>12.228070175438598</v>
+        <v>9.6192237328526478</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
@@ -1047,7 +1065,7 @@
       </c>
       <c r="D9" s="1">
         <f>D5*C9+D6</f>
-        <v>8.5</v>
+        <v>7.1200639149430209</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
@@ -1059,7 +1077,7 @@
       </c>
       <c r="D10" s="1">
         <f>(C10-D6)/D5</f>
-        <v>2.5000000000000004</v>
+        <v>1.1196000000000004</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
@@ -1070,17 +1088,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="1">
-        <f>(E3-E2)/(D3-D2)</f>
-        <v>1</v>
+        <f>(E3-E2)/(C3-C2)</f>
+        <v>0.97799511002444983</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1">
-        <f>D2</f>
-        <v>8.1999999999999993</v>
+        <f>C2</f>
+        <v>8.5</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
@@ -1089,7 +1107,7 @@
       </c>
       <c r="D14" s="1">
         <f>E2</f>
-        <v>8.1999999999999993</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
@@ -1112,7 +1130,128 @@
       </c>
       <c r="D16" s="1">
         <f>(C16-D2)*D5+E2</f>
-        <v>8.1999999999999993</v>
+        <v>1.3219795301090711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <f>(D20-$D$13)*$D$12+$D$14</f>
+        <v>8.5169289053191157</v>
+      </c>
+      <c r="D20" s="3">
+        <f>B20*$D$5+$D$6</f>
+        <v>8.6195598056887963</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="2">
+        <v>1.1195999999999999</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" ref="C21:C27" si="0">(D21-$D$13)*$D$12+$D$14</f>
+        <v>8.4</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" ref="D21:D27" si="1">B21*$D$5+$D$6</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>6.561596040450949</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="1"/>
+        <v>6.6202319513610952</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>5.5839296080168648</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>5.6205680241972438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>4.6062631755827805</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>4.6209040970333932</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>3.6285967431486972</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="1"/>
+        <v>3.6212401698695427</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="2">
+        <v>7.6657999999999999</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="1"/>
+        <v>1.9559999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6732638782805296</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6219123155418407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Read Test Vector utility
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00788a1fe100dfc/Documents/GitHub/PWC-OLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D2C35F2-EE84-41DD-B607-3C2E5EC3A0A9}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACBC370D-84AF-4525-8B18-9DD0500DB05A}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1780" windowWidth="17180" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="1220" yWindow="1720" windowWidth="17180" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
+    <sheet name="Cal_4-30" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>M</t>
   </si>
@@ -82,15 +83,6 @@
     <t>LKe</t>
   </si>
   <si>
-    <t>Level Scaled</t>
-  </si>
-  <si>
-    <t>Level Keyence</t>
-  </si>
-  <si>
-    <t>Level Reference</t>
-  </si>
-  <si>
     <t>Empty (Low)</t>
   </si>
   <si>
@@ -128,14 +120,36 @@
   </si>
   <si>
     <t>Full</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Lk (Raw)</t>
+  </si>
+  <si>
+    <t>Lm</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Lk</t>
+  </si>
+  <si>
+    <t>Pve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -172,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -181,6 +195,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -323,13 +345,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>M = (LSf -LSe) /  (LKf -LKe)</a:t>
+            <a:t>M = (Lmf -Lme) /  (LKf -LKe)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>B = LSe - M * LKe</a:t>
+            <a:t>B = Lme - M * LKe</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -377,7 +399,10 @@
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>m</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -488,16 +513,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -512,7 +537,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5829300" y="1085850"/>
+          <a:off x="5676900" y="1835150"/>
           <a:ext cx="2940050" cy="1504950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -639,6 +664,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3BA94E-7FD5-4678-9436-02C8EAFB1FBB}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -970,29 +999,29 @@
     <col min="3" max="6" width="9.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="C2" s="7">
         <v>8.5</v>
       </c>
-      <c r="D2" s="2">
-        <v>1.1195999999999999</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8.4</v>
+      <c r="D2" s="7">
+        <v>1.111</v>
+      </c>
+      <c r="E2" s="7">
+        <v>8.48</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -1001,21 +1030,39 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.956</v>
-      </c>
-      <c r="D3" s="2">
-        <v>7.6657999999999999</v>
-      </c>
-      <c r="E3" s="2">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
         <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>7.6539999999999999</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.903</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -1026,8 +1073,53 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>8.5</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1.1105</v>
+      </c>
+      <c r="N3" s="6">
+        <v>8.48</v>
+      </c>
+      <c r="O3" s="6">
+        <f>N3-Q3</f>
+        <v>-5.0259819654741023E-4</v>
+      </c>
+      <c r="P3" s="6">
+        <v>8.5050000000000008</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>$D$5*M3+$D$6</f>
+        <v>8.4805025981965478</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="M4" s="6">
+        <v>2.6190000000000002</v>
+      </c>
+      <c r="N4" s="6">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="O4" s="6">
+        <f t="shared" ref="O4:O7" si="0">N4-Q4</f>
+        <v>1.8361607825152504E-3</v>
+      </c>
+      <c r="P4" s="6">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" ref="Q4:Q7" si="1">$D$5*M4+$D$6</f>
+        <v>6.9641638392174849</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1035,82 +1127,147 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f>(C3-C2)/(D3-D2)</f>
-        <v>-0.99966392716385089</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+        <f>(E3-E2)/(D3-D2)</f>
+        <v>-1.0051963930918539</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5" s="6">
+        <v>4.6319999999999997</v>
+      </c>
+      <c r="N5" s="6">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.0349992358309521E-4</v>
+      </c>
+      <c r="P5" s="6">
+        <v>5.0129999999999999</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" si="1"/>
+        <v>4.9407034999235835</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <f>C2-D5*D2</f>
-        <v>9.6192237328526478</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+        <f>E2-D5*D2</f>
+        <v>9.5967731927250508</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6.6449999999999996</v>
+      </c>
+      <c r="N6" s="6">
+        <v>2.915</v>
+      </c>
+      <c r="O6" s="6">
+        <f t="shared" si="0"/>
+        <v>-2.243160629681995E-3</v>
+      </c>
+      <c r="P6" s="6">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="Q6" s="5">
+        <f t="shared" si="1"/>
+        <v>2.917243160629682</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1.903</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="0"/>
+        <v>-2.0103927861847559E-3</v>
+      </c>
+      <c r="P7" s="6">
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="Q7" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9050103927861848</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2">
         <v>2.5</v>
       </c>
       <c r="D9" s="1">
         <f>D5*C9+D6</f>
-        <v>7.1200639149430209</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+        <v>7.083782209995416</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
         <f>(C10-D6)/D5</f>
-        <v>1.1196000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+        <v>1.0911033906036198</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <f>(E3-E2)/(C3-C2)</f>
-        <v>0.97799511002444983</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+        <v>1.0118461538461538</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <f>C2</f>
         <v>8.5</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
         <f>E2</f>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1121,21 +1278,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
         <v>8.1999999999999993</v>
       </c>
       <c r="D16" s="1">
         <f>(C16-D2)*D5+E2</f>
-        <v>1.3219795301090711</v>
+        <v>1.3541627693718485</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -1146,18 +1303,18 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="3">
         <f>(D20-$D$13)*$D$12+$D$14</f>
-        <v>8.5169289053191157</v>
+        <v>8.5726616324903908</v>
       </c>
       <c r="D20" s="3">
         <f>B20*$D$5+$D$6</f>
-        <v>8.6195598056887963</v>
+        <v>8.5915767996331969</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1165,12 +1322,12 @@
         <v>1.1195999999999999</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" ref="C21:C27" si="0">(D21-$D$13)*$D$12+$D$14</f>
-        <v>8.4</v>
+        <f t="shared" ref="C21:C27" si="2">(D21-$D$13)*$D$12+$D$14</f>
+        <v>8.451015981626874</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" ref="D21:D27" si="1">B21*$D$5+$D$6</f>
-        <v>8.5</v>
+        <f t="shared" ref="D21:D27" si="3">B21*$D$5+$D$6</f>
+        <v>8.471355311019412</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1178,12 +1335,12 @@
         <v>3</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="0"/>
-        <v>6.561596040450949</v>
+        <f t="shared" si="2"/>
+        <v>6.5384534240703527</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="1"/>
-        <v>6.6202319513610952</v>
+        <f t="shared" si="3"/>
+        <v>6.581184013449489</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1191,12 +1348,12 @@
         <v>4</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="0"/>
-        <v>5.5839296080168648</v>
+        <f t="shared" si="2"/>
+        <v>5.5213493198603336</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="1"/>
-        <v>5.6205680241972438</v>
+        <f t="shared" si="3"/>
+        <v>5.5759876203576351</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1204,12 +1361,12 @@
         <v>5</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="0"/>
-        <v>4.6062631755827805</v>
+        <f t="shared" si="2"/>
+        <v>4.5042452156503145</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="1"/>
-        <v>4.6209040970333932</v>
+        <f t="shared" si="3"/>
+        <v>4.5707912272657811</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1217,12 +1374,12 @@
         <v>6</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="0"/>
-        <v>3.6285967431486972</v>
+        <f t="shared" si="2"/>
+        <v>3.4871411114402955</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="1"/>
-        <v>3.6212401698695427</v>
+        <f t="shared" si="3"/>
+        <v>3.5655948341739272</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -1230,32 +1387,154 @@
         <v>7.6657999999999999</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.7928490946472468</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="1"/>
-        <v>1.9559999999999995</v>
+        <f t="shared" si="3"/>
+        <v>1.8911386825615173</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>8</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6732638782805296</v>
+        <f t="shared" si="2"/>
+        <v>1.4529329030202573</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="1"/>
-        <v>1.6219123155418407</v>
+        <f t="shared" si="3"/>
+        <v>1.5552020479902193</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBEE94-87B5-4FED-946A-4BC9514D2347}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCellId="2" sqref="A7:E7 A6:D6 A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>8.5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>8.5050000000000008</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.1105</v>
+      </c>
+      <c r="D2" s="6">
+        <v>8.48</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2-B2</f>
+        <v>-2.5000000000000355E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.6190000000000002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E6" si="0">D3-B3</f>
+        <v>-4.8000000000000043E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5.0129999999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4.6319999999999997</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.299999999999951E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="C5" s="6">
+        <v>6.6449999999999996</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.915</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>-9.7999999999999865E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.903</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.10999999999999988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Contains the Read vector and LUT bug fix.
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00788a1fe100dfc/Documents/GitHub/PWC-OLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACBC370D-84AF-4525-8B18-9DD0500DB05A}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="680" windowWidth="15780" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="1220" yWindow="1720" windowWidth="17180" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tank Calibrations" sheetId="1" r:id="rId1"/>
+    <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
+    <sheet name="Cal_4-30" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="LKe">'Tank Calibrations'!$D$2</definedName>
-    <definedName name="LKf">'Tank Calibrations'!$D$3</definedName>
-    <definedName name="LMe">'Tank Calibrations'!$E$2</definedName>
-    <definedName name="LMf">'Tank Calibrations'!$E$3</definedName>
-    <definedName name="LSe">'Tank Calibrations'!$C$2</definedName>
-    <definedName name="LSf">'Tank Calibrations'!$C$3</definedName>
+    <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
+    <definedName name="LKf">'Level Calibrations'!$D$3</definedName>
+    <definedName name="LMe">'Level Calibrations'!$E$2</definedName>
+    <definedName name="LMf">'Level Calibrations'!$E$3</definedName>
+    <definedName name="LSe">'Level Calibrations'!$C$2</definedName>
+    <definedName name="LSf">'Level Calibrations'!$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>M</t>
   </si>
@@ -82,15 +83,6 @@
     <t>LKe</t>
   </si>
   <si>
-    <t>Level Scaled</t>
-  </si>
-  <si>
-    <t>Level Keyence</t>
-  </si>
-  <si>
-    <t>Level Reference</t>
-  </si>
-  <si>
     <t>Empty (Low)</t>
   </si>
   <si>
@@ -116,12 +108,49 @@
   </si>
   <si>
     <t>LK (key raw)</t>
+  </si>
+  <si>
+    <t>Lse</t>
+  </si>
+  <si>
+    <t>Key Measure</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Lk (Raw)</t>
+  </si>
+  <si>
+    <t>Lm</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Lk</t>
+  </si>
+  <si>
+    <t>Pve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,12 +186,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -305,13 +345,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>M = (LSf -LSe) /  (LKf -LKe)</a:t>
+            <a:t>M = (Lmf -Lme) /  (LKf -LKe)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>B = LSe - M * LKe</a:t>
+            <a:t>B = Lme - M * LKe</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -359,7 +399,10 @@
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>m</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -428,7 +471,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Mc = (LMf -LMe) /  (LKf -LKe)</a:t>
+            <a:t>Mc = (LMf -LMe) /  (LSf -LSe)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -470,16 +513,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -494,7 +537,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5829300" y="1085850"/>
+          <a:off x="5676900" y="1835150"/>
           <a:ext cx="2940050" cy="1504950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -621,6 +664,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -940,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3BA94E-7FD5-4678-9436-02C8EAFB1FBB}">
-  <dimension ref="B1:J16"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -952,29 +999,29 @@
     <col min="3" max="6" width="9.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8.1999999999999993</v>
+      <c r="C2" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.111</v>
+      </c>
+      <c r="E2" s="7">
+        <v>8.48</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -983,21 +1030,39 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2.5</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>7.6539999999999999</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.903</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -1008,8 +1073,53 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>8.5</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1.1105</v>
+      </c>
+      <c r="N3" s="6">
+        <v>8.48</v>
+      </c>
+      <c r="O3" s="6">
+        <f>N3-Q3</f>
+        <v>-5.0259819654741023E-4</v>
+      </c>
+      <c r="P3" s="6">
+        <v>8.5050000000000008</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>$D$5*M3+$D$6</f>
+        <v>8.4805025981965478</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="M4" s="6">
+        <v>2.6190000000000002</v>
+      </c>
+      <c r="N4" s="6">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="O4" s="6">
+        <f t="shared" ref="O4:O7" si="0">N4-Q4</f>
+        <v>1.8361607825152504E-3</v>
+      </c>
+      <c r="P4" s="6">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" ref="Q4:Q7" si="1">$D$5*M4+$D$6</f>
+        <v>6.9641638392174849</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1017,82 +1127,147 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f>(C3-C2)/(D3-D2)</f>
-        <v>-1.4912280701754388</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+        <f>(E3-E2)/(D3-D2)</f>
+        <v>-1.0051963930918539</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5" s="6">
+        <v>4.6319999999999997</v>
+      </c>
+      <c r="N5" s="6">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.0349992358309521E-4</v>
+      </c>
+      <c r="P5" s="6">
+        <v>5.0129999999999999</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" si="1"/>
+        <v>4.9407034999235835</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <f>C2-D5*D2</f>
-        <v>12.228070175438598</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+        <f>E2-D5*D2</f>
+        <v>9.5967731927250508</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6.6449999999999996</v>
+      </c>
+      <c r="N6" s="6">
+        <v>2.915</v>
+      </c>
+      <c r="O6" s="6">
+        <f t="shared" si="0"/>
+        <v>-2.243160629681995E-3</v>
+      </c>
+      <c r="P6" s="6">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="Q6" s="5">
+        <f t="shared" si="1"/>
+        <v>2.917243160629682</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1.903</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="0"/>
+        <v>-2.0103927861847559E-3</v>
+      </c>
+      <c r="P7" s="6">
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="Q7" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9050103927861848</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2">
         <v>2.5</v>
       </c>
       <c r="D9" s="1">
         <f>D5*C9+D6</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+        <v>7.083782209995416</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
         <f>(C10-D6)/D5</f>
-        <v>2.5000000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+        <v>1.0911033906036198</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1">
+        <f>(E3-E2)/(C3-C2)</f>
+        <v>1.0118461538461538</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1">
-        <f>(E3-E2)/(D3-D2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D13" s="1">
-        <f>D2</f>
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+        <f>C2</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
         <f>E2</f>
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1103,20 +1278,263 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
         <v>8.1999999999999993</v>
       </c>
       <c r="D16" s="1">
         <f>(C16-D2)*D5+E2</f>
-        <v>8.1999999999999993</v>
+        <v>1.3541627693718485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <f>(D20-$D$13)*$D$12+$D$14</f>
+        <v>8.5726616324903908</v>
+      </c>
+      <c r="D20" s="3">
+        <f>B20*$D$5+$D$6</f>
+        <v>8.5915767996331969</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="2">
+        <v>1.1195999999999999</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" ref="C21:C27" si="2">(D21-$D$13)*$D$12+$D$14</f>
+        <v>8.451015981626874</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" ref="D21:D27" si="3">B21*$D$5+$D$6</f>
+        <v>8.471355311019412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>6.5384534240703527</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="3"/>
+        <v>6.581184013449489</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
+        <v>5.5213493198603336</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="3"/>
+        <v>5.5759876203576351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>4.5042452156503145</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="3"/>
+        <v>4.5707912272657811</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4871411114402955</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="3"/>
+        <v>3.5655948341739272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="2">
+        <v>7.6657999999999999</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
+        <v>1.7928490946472468</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="3"/>
+        <v>1.8911386825615173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4529329030202573</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5552020479902193</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBEE94-87B5-4FED-946A-4BC9514D2347}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCellId="2" sqref="A7:E7 A6:D6 A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>8.5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>8.5050000000000008</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.1105</v>
+      </c>
+      <c r="D2" s="6">
+        <v>8.48</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2-B2</f>
+        <v>-2.5000000000000355E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.6190000000000002</v>
+      </c>
+      <c r="D3" s="6">
+        <v>6.9660000000000002</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E6" si="0">D3-B3</f>
+        <v>-4.8000000000000043E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5.0129999999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4.6319999999999997</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.299999999999951E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.0129999999999999</v>
+      </c>
+      <c r="C5" s="6">
+        <v>6.6449999999999996</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.915</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>-9.7999999999999865E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.903</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.10999999999999988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fist exe application build, had to install VISA runtime on the target PC.  Still need to load Keyance sensors.
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00788a1fe100dfc/Documents/GitHub/PWC-OLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACBC370D-84AF-4525-8B18-9DD0500DB05A}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D131884F-DC08-4906-A406-3805B69E0AA9}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="1720" windowWidth="17180" windowHeight="10310" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView minimized="1" xWindow="1420" yWindow="490" windowWidth="17780" windowHeight="8350" activeTab="1" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
-    <sheet name="Cal_4-30" sheetId="2" r:id="rId2"/>
+    <sheet name="Cal New 6-18" sheetId="3" r:id="rId2"/>
+    <sheet name="Cal_4-30" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>M</t>
   </si>
@@ -222,6 +223,946 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cal New 6-18'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.20348556430446188"/>
+                  <c:y val="2.8516331291921843E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Cal New 6-18'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.7195</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3540999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7796000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4389000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0039999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0781999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Cal New 6-18'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.9020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5419999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0FD5-4EDF-9014-4BC2D02F2803}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1239171919"/>
+        <c:axId val="1239173839"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1239171919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1239173839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1239173839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1239171919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -666,8 +1607,45 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165106</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B807B51-9FDB-95CC-A936-6F0F2649AA86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -989,7 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3BA94E-7FD5-4678-9436-02C8EAFB1FBB}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
@@ -1418,6 +2396,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D438230-A6A4-489E-9116-8D7FE61726C4}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>4.7195</v>
+      </c>
+      <c r="B2">
+        <v>4.9020000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5.3540999999999999</v>
+      </c>
+      <c r="B3">
+        <v>4.2690000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5.7796000000000003</v>
+      </c>
+      <c r="B4">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6.4389000000000003</v>
+      </c>
+      <c r="B5">
+        <v>3.1890000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>7.0039999999999996</v>
+      </c>
+      <c r="B6">
+        <v>2.6190000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4.0781999999999998</v>
+      </c>
+      <c r="B7">
+        <v>5.5419999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBEE94-87B5-4FED-946A-4BC9514D2347}">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Major updates to the state machine, basically working, the Drain Level check are not working, probably due to 3 second pause makes so drain switch can nolonger indicate drain mode.
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00788a1fe100dfc/Documents/GitHub/PWC-OLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\OLS Level Test Project\PWC-OLS-Rev2\PWC-OLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{F6BE86C3-B46D-4EF2-9CEA-260A294ACED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D131884F-DC08-4906-A406-3805B69E0AA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D66FC19-63E7-4CB1-A8C8-37C4DC597F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1420" yWindow="490" windowWidth="17780" windowHeight="8350" activeTab="1" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="2430" yWindow="0" windowWidth="21555" windowHeight="13440" activeTab="2" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
     <sheet name="Cal New 6-18" sheetId="3" r:id="rId2"/>
-    <sheet name="Cal_4-30" sheetId="2" r:id="rId3"/>
+    <sheet name="PWM" sheetId="4" r:id="rId3"/>
+    <sheet name="Cal_4-30" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>M</t>
   </si>
@@ -142,17 +143,54 @@
   </si>
   <si>
     <t>Pve</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Ton</t>
+  </si>
+  <si>
+    <t>Toff</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency </t>
+  </si>
+  <si>
+    <t>Duty Cycle</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Rsub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,10 +222,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,9 +246,16 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1648,6 +1695,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>399559</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9528E42-9419-00C4-7866-EA6B1D39756A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6829425" y="476249"/>
+          <a:ext cx="4600084" cy="2924175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47754</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>55828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4753EFF-703F-C806-B0A7-3032F5EEB8BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7943850" y="3095754"/>
+          <a:ext cx="3638550" cy="3246574"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1971,13 +2111,13 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="6" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1988,7 +2128,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -2029,7 +2169,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2075,7 +2215,7 @@
         <v>8.4805025981965478</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="L4">
         <v>7</v>
       </c>
@@ -2097,7 +2237,7 @@
         <v>6.9641638392174849</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -2129,7 +2269,7 @@
         <v>4.9407034999235835</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2158,7 +2298,7 @@
         <v>2.917243160629682</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
         <v>24</v>
       </c>
@@ -2183,7 +2323,7 @@
         <v>1.9050103927861848</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2191,7 +2331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2203,7 +2343,7 @@
         <v>7.083782209995416</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -2215,7 +2355,7 @@
         <v>1.0911033906036198</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -2227,7 +2367,7 @@
         <v>1.0118461538461538</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
@@ -2236,7 +2376,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2245,7 +2385,7 @@
         <v>8.48</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -2256,7 +2396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -2268,7 +2408,7 @@
         <v>1.3541627693718485</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -2279,7 +2419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2295,7 +2435,7 @@
         <v>8.5915767996331969</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>1.1195999999999999</v>
       </c>
@@ -2308,7 +2448,7 @@
         <v>8.471355311019412</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>3</v>
       </c>
@@ -2321,7 +2461,7 @@
         <v>6.581184013449489</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>4</v>
       </c>
@@ -2334,7 +2474,7 @@
         <v>5.5759876203576351</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>5</v>
       </c>
@@ -2347,7 +2487,7 @@
         <v>4.5707912272657811</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>6</v>
       </c>
@@ -2360,7 +2500,7 @@
         <v>3.5655948341739272</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>7.6657999999999999</v>
       </c>
@@ -2373,7 +2513,7 @@
         <v>1.8911386825615173</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2399,13 +2539,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D438230-A6A4-489E-9116-8D7FE61726C4}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2413,7 +2553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.7195</v>
       </c>
@@ -2421,7 +2561,7 @@
         <v>4.9020000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.3540999999999999</v>
       </c>
@@ -2429,7 +2569,7 @@
         <v>4.2690000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.7796000000000003</v>
       </c>
@@ -2437,7 +2577,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.4389000000000003</v>
       </c>
@@ -2445,7 +2585,7 @@
         <v>3.1890000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.0039999999999996</v>
       </c>
@@ -2453,7 +2593,7 @@
         <v>2.6190000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.0781999999999998</v>
       </c>
@@ -2468,6 +2608,324 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35334F14-13A4-4C34-95A2-5D594844CE43}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="8">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D2" s="8">
+        <f>0.693*(A2+B2)*$C$2</f>
+        <v>7.6229999999999997E-6</v>
+      </c>
+      <c r="E2" s="8">
+        <f>0.693*B2*$C$2</f>
+        <v>6.9299999999999997E-6</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2+E2</f>
+        <v>1.4552999999999999E-5</v>
+      </c>
+      <c r="G2" s="10">
+        <f>1/F2</f>
+        <v>68714.354428640145</v>
+      </c>
+      <c r="H2" s="11">
+        <f>D2/(D2+E2)*100</f>
+        <v>52.380952380952387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>10000</v>
+      </c>
+      <c r="B3" s="8">
+        <v>100000</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D4" si="0">0.693*(A3+B3)*$C$2</f>
+        <v>7.6230000000000007E-5</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E4" si="1">0.693*B3*$C$2</f>
+        <v>6.9300000000000004E-5</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F4" si="2">D3+E3</f>
+        <v>1.4553E-4</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G4" si="3">1/F3</f>
+        <v>6871.4354428640145</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" ref="H3:H4" si="4">D3/(D3+E3)*100</f>
+        <v>52.380952380952387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <f>A7</f>
+        <v>28799.999999999996</v>
+      </c>
+      <c r="B4" s="8">
+        <f>B7</f>
+        <v>28799.999999999996</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>3.9916799999999997E-5</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="1"/>
+        <v>1.9958399999999999E-5</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="2"/>
+        <v>5.9875199999999992E-5</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="3"/>
+        <v>16701.405590294482</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="4"/>
+        <v>66.666666666666671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="8">
+        <f>1/C2</f>
+        <v>999999999.99999988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <f>D7-B7</f>
+        <v>28799.999999999996</v>
+      </c>
+      <c r="B7" s="8">
+        <f>D7/A6</f>
+        <v>28799.999999999996</v>
+      </c>
+      <c r="D7" s="9">
+        <f>1.44/G7/$C$2</f>
+        <v>57599.999999999993</v>
+      </c>
+      <c r="F7" s="8">
+        <f>1/G7</f>
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="G7" s="10">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="D9" s="12">
+        <f>(A9+B9)/(A9+2*B9)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" ref="D10:D20" si="5">(A10+B10)/(A10+2*B10)</f>
+        <v>0.52380952380952384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="5"/>
+        <v>0.65517241379310343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="5"/>
+        <v>0.69696969696969702</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>170</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="5"/>
+        <v>0.72972972972972971</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>210</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="5"/>
+        <v>0.75609756097560976</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>250</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="5"/>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>290</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="5"/>
+        <v>0.79591836734693877</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>330</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="5"/>
+        <v>0.81132075471698117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>370</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="5"/>
+        <v>0.82456140350877194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>100000000</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="D20" s="12">
+        <f t="shared" si="5"/>
+        <v>0.99999900000200004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBEE94-87B5-4FED-946A-4BC9514D2347}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2475,9 +2933,9 @@
       <selection activeCellId="2" sqref="A7:E7 A6:D6 A1:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -2494,7 +2952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8.5</v>
       </c>
@@ -2512,7 +2970,7 @@
         <v>-2.5000000000000355E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -2530,7 +2988,7 @@
         <v>-4.8000000000000043E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -2548,7 +3006,7 @@
         <v>-7.299999999999951E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2566,7 +3024,7 @@
         <v>-9.7999999999999865E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Added ATP Spec definition, change the Pump speed control for 4 speeds, Stop, Creep, Slow & Fast
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\OLS Level Test Project\PWC-OLS-Rev2\PWC-OLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PWC-OLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D66FC19-63E7-4CB1-A8C8-37C4DC597F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D525F93A-D435-48C3-908E-6CE885C25BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="0" windowWidth="21555" windowHeight="13440" activeTab="2" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="410" yWindow="1140" windowWidth="18790" windowHeight="9460" activeTab="2" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
     <sheet name="Cal New 6-18" sheetId="3" r:id="rId2"/>
     <sheet name="PWM" sheetId="4" r:id="rId3"/>
-    <sheet name="Cal_4-30" sheetId="2" r:id="rId4"/>
+    <sheet name="Juml" sheetId="5" r:id="rId4"/>
+    <sheet name="Cal_4-30" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>M</t>
   </si>
@@ -170,6 +171,27 @@
   </si>
   <si>
     <t>Rsub</t>
+  </si>
+  <si>
+    <t>Ton = R1 + R2</t>
+  </si>
+  <si>
+    <t>T = R1 +2R2</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Creep</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Stop</t>
   </si>
 </sst>
 </file>
@@ -180,8 +202,8 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -227,7 +249,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -248,9 +270,10 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2111,13 +2134,13 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="6" width="9.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2128,7 +2151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -2169,7 +2192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2215,7 +2238,7 @@
         <v>8.4805025981965478</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="L4">
         <v>7</v>
       </c>
@@ -2237,7 +2260,7 @@
         <v>6.9641638392174849</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -2269,7 +2292,7 @@
         <v>4.9407034999235835</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2321,7 @@
         <v>2.917243160629682</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="K7" t="s">
         <v>24</v>
       </c>
@@ -2323,7 +2346,7 @@
         <v>1.9050103927861848</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2331,7 +2354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2343,7 +2366,7 @@
         <v>7.083782209995416</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -2355,7 +2378,7 @@
         <v>1.0911033906036198</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -2367,7 +2390,7 @@
         <v>1.0118461538461538</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
@@ -2376,7 +2399,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2385,7 +2408,7 @@
         <v>8.48</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -2396,7 +2419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -2408,7 +2431,7 @@
         <v>1.3541627693718485</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -2419,7 +2442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2435,7 +2458,7 @@
         <v>8.5915767996331969</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>1.1195999999999999</v>
       </c>
@@ -2448,7 +2471,7 @@
         <v>8.471355311019412</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>3</v>
       </c>
@@ -2461,7 +2484,7 @@
         <v>6.581184013449489</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>4</v>
       </c>
@@ -2474,7 +2497,7 @@
         <v>5.5759876203576351</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>5</v>
       </c>
@@ -2487,7 +2510,7 @@
         <v>4.5707912272657811</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>6</v>
       </c>
@@ -2500,7 +2523,7 @@
         <v>3.5655948341739272</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B26" s="2">
         <v>7.6657999999999999</v>
       </c>
@@ -2513,7 +2536,7 @@
         <v>1.8911386825615173</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2543,9 +2566,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2553,7 +2576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4.7195</v>
       </c>
@@ -2561,7 +2584,7 @@
         <v>4.9020000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5.3540999999999999</v>
       </c>
@@ -2569,7 +2592,7 @@
         <v>4.2690000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5.7796000000000003</v>
       </c>
@@ -2577,7 +2600,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6.4389000000000003</v>
       </c>
@@ -2585,7 +2608,7 @@
         <v>3.1890000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>7.0039999999999996</v>
       </c>
@@ -2593,7 +2616,7 @@
         <v>2.6190000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4.0781999999999998</v>
       </c>
@@ -2609,22 +2632,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35334F14-13A4-4C34-95A2-5D594844CE43}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2650,7 +2673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>1000</v>
       </c>
@@ -2681,7 +2704,7 @@
         <v>52.380952380952387</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>10000</v>
       </c>
@@ -2710,7 +2733,7 @@
         <v>52.380952380952387</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <f>A7</f>
         <v>28799.999999999996</v>
@@ -2741,7 +2764,7 @@
         <v>66.666666666666671</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2753,7 +2776,7 @@
         <v>999999999.99999988</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <f>D7-B7</f>
         <v>28799.999999999996</v>
@@ -2774,7 +2797,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2786,7 +2809,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2798,7 +2821,7 @@
         <v>0.52380952380952384</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>50</v>
       </c>
@@ -2810,7 +2833,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>90</v>
       </c>
@@ -2822,7 +2845,7 @@
         <v>0.65517241379310343</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>130</v>
       </c>
@@ -2834,7 +2857,7 @@
         <v>0.69696969696969702</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>170</v>
       </c>
@@ -2846,7 +2869,7 @@
         <v>0.72972972972972971</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>210</v>
       </c>
@@ -2858,7 +2881,7 @@
         <v>0.75609756097560976</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>250</v>
       </c>
@@ -2870,7 +2893,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>290</v>
       </c>
@@ -2882,7 +2905,7 @@
         <v>0.79591836734693877</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>330</v>
       </c>
@@ -2894,7 +2917,7 @@
         <v>0.81132075471698117</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>370</v>
       </c>
@@ -2906,7 +2929,7 @@
         <v>0.82456140350877194</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>100000000</v>
       </c>
@@ -2917,6 +2940,118 @@
         <f t="shared" si="5"/>
         <v>0.99999900000200004</v>
       </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D27">
+        <v>2200</v>
+      </c>
+      <c r="E27" s="13">
+        <f>C27+D27</f>
+        <v>12200</v>
+      </c>
+      <c r="F27">
+        <f>C27+2*D27</f>
+        <v>14400</v>
+      </c>
+      <c r="G27">
+        <f>E27/F27</f>
+        <v>0.84722222222222221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28">
+        <v>750</v>
+      </c>
+      <c r="D28">
+        <v>10000</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" ref="E28:E30" si="6">C28+D28</f>
+        <v>10750</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F30" si="7">C28+2*D28</f>
+        <v>20750</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="8">E28/F28</f>
+        <v>0.51807228915662651</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>4777</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="6"/>
+        <v>4777</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>9554</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30">
+        <v>4700</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="6"/>
+        <v>4700</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="7"/>
+        <v>4700</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2926,6 +3061,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3006B20C-4981-41FD-AD8F-C57648615C1B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBEE94-87B5-4FED-946A-4BC9514D2347}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2933,9 +3082,9 @@
       <selection activeCellId="2" sqref="A7:E7 A6:D6 A1:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -2952,7 +3101,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8.5</v>
       </c>
@@ -2970,7 +3119,7 @@
         <v>-2.5000000000000355E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7</v>
       </c>
@@ -2988,7 +3137,7 @@
         <v>-4.8000000000000043E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
@@ -3006,7 +3155,7 @@
         <v>-7.299999999999951E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3024,7 +3173,7 @@
         <v>-9.7999999999999865E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
added double transition err check
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PWC-OLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D525F93A-D435-48C3-908E-6CE885C25BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2492F6EA-C9E3-4DD5-BFDF-884E2DDE5FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="410" yWindow="1140" windowWidth="18790" windowHeight="9460" activeTab="2" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="-90" yWindow="380" windowWidth="19380" windowHeight="9460" activeTab="3" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
     <sheet name="Cal New 6-18" sheetId="3" r:id="rId2"/>
     <sheet name="PWM" sheetId="4" r:id="rId3"/>
-    <sheet name="Juml" sheetId="5" r:id="rId4"/>
-    <sheet name="Cal_4-30" sheetId="2" r:id="rId5"/>
+    <sheet name="3092 I-source" sheetId="6" r:id="rId4"/>
+    <sheet name="Juml" sheetId="5" r:id="rId5"/>
+    <sheet name="Cal_4-30" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>M</t>
   </si>
@@ -192,6 +193,24 @@
   </si>
   <si>
     <t>Stop</t>
+  </si>
+  <si>
+    <t>Iout =10uA *(Rset/Rout+1)</t>
+  </si>
+  <si>
+    <t>Rset</t>
+  </si>
+  <si>
+    <t>Rout</t>
+  </si>
+  <si>
+    <t>Iout</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>ratio =  R1/(R1+R2)</t>
   </si>
 </sst>
 </file>
@@ -2634,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35334F14-13A4-4C34-95A2-5D594844CE43}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3061,6 +3080,72 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F764E4-5102-4DB7-8EE3-2F288C2743C0}">
+  <dimension ref="B3:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C6">
+        <v>20000</v>
+      </c>
+      <c r="D6">
+        <f>0.00001/(B6-0.00001)*C6</f>
+        <v>25.031289111389238</v>
+      </c>
+      <c r="E6">
+        <f>9/(0.014*1200)</f>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5600000</v>
+      </c>
+      <c r="G6" s="8">
+        <f>F6/E6-F6</f>
+        <v>4853333.333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3006B20C-4981-41FD-AD8F-C57648615C1B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3074,7 +3159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FBEE94-87B5-4FED-946A-4BC9514D2347}">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Has the tank rate measurement with 18v7 controller
</commit_message>
<xml_diff>
--- a/Calculations Reference.xlsx
+++ b/Calculations Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PWC-OLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782021B3-68B3-43B8-8F7D-5AA813D903F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B00D42C-00FE-49E6-A44D-E269DF4040CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="10" windowWidth="19200" windowHeight="11240" firstSheet="1" activeTab="7" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
+    <workbookView xWindow="4800" yWindow="1030" windowWidth="5950" windowHeight="11240" firstSheet="2" activeTab="8" xr2:uid="{726BA5CB-03EF-4BFF-90D1-A26922DC8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Level Calibrations" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,11 @@
     <sheet name="Cal_4-30" sheetId="2" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
     <sheet name="TU5" sheetId="8" r:id="rId8"/>
+    <sheet name="Tank Rate 10-10" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'TU5'!$M$91:$M$210</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'TU5'!$N$91:$N$210</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'TU5'!$K$91:$K$210</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'TU5'!$L$91:$L$210</definedName>
     <definedName name="LKe">'Level Calibrations'!$D$2</definedName>
     <definedName name="LKf">'Level Calibrations'!$D$3</definedName>
     <definedName name="LMe">'Level Calibrations'!$E$2</definedName>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="105">
   <si>
     <t>M</t>
   </si>
@@ -328,6 +327,48 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>F100%</t>
+  </si>
+  <si>
+    <t>Amps</t>
+  </si>
+  <si>
+    <t>in/sec</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>D100%</t>
+  </si>
+  <si>
+    <t>D50%</t>
+  </si>
+  <si>
+    <t>F50%</t>
+  </si>
+  <si>
+    <t>D25%</t>
+  </si>
+  <si>
+    <t>F25%</t>
+  </si>
+  <si>
+    <t>D10%</t>
+  </si>
+  <si>
+    <t>D2%</t>
+  </si>
+  <si>
+    <t>D5%</t>
+  </si>
+  <si>
+    <t>F5%</t>
+  </si>
+  <si>
+    <t>F2%</t>
   </si>
 </sst>
 </file>
@@ -8020,7 +8061,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4594225" y="35998150"/>
+              <a:off x="5832475" y="35998150"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -10554,7 +10595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E556B2-B3CA-41A3-B01F-E2D3945E563F}">
   <dimension ref="A1:Y235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+    <sheetView topLeftCell="A160" workbookViewId="0">
       <selection activeCell="Q154" sqref="Q154"/>
     </sheetView>
   </sheetViews>
@@ -16417,4 +16458,695 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48B72D3-4694-4AC1-AFEE-1C308B28D022}">
+  <dimension ref="A1:D71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="8.7265625" style="14"/>
+    <col min="4" max="4" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="11">
+        <v>8</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2.65</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5.11E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="11">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14">
+        <v>-2.65</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-5.0700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="11">
+        <v>7</v>
+      </c>
+      <c r="C4" s="14">
+        <v>-2.65</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-4.9700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="11">
+        <v>5</v>
+      </c>
+      <c r="C5" s="14">
+        <v>-2.65</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-4.99E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="11">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>-2.66</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-4.99E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2.64</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2.64</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4.99E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="11">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2.64</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="11">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14">
+        <v>-1.5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>-2.52E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14">
+        <v>-1.49</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-2.47E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="11">
+        <v>5</v>
+      </c>
+      <c r="C12" s="14">
+        <v>-1.48</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-2.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="11">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14">
+        <v>-1.48</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-2.47E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1.35</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2.5600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="11">
+        <v>5</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1.37</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="11">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1.38</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2.5399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="11">
+        <v>8</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1.38</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2.5899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="11">
+        <v>8.5</v>
+      </c>
+      <c r="C18" s="14">
+        <v>-0.95</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="11">
+        <v>7</v>
+      </c>
+      <c r="C19" s="14">
+        <v>-0.86</v>
+      </c>
+      <c r="D19" s="5">
+        <v>-1.21E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="11">
+        <v>5</v>
+      </c>
+      <c r="C20" s="14">
+        <v>-0.86</v>
+      </c>
+      <c r="D20" s="5">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3</v>
+      </c>
+      <c r="C21" s="14">
+        <v>-0.86</v>
+      </c>
+      <c r="D21" s="5">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="11">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0.78</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="11">
+        <v>5</v>
+      </c>
+      <c r="C23" s="14">
+        <v>0.78</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1.24E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="11">
+        <v>7</v>
+      </c>
+      <c r="C24" s="14">
+        <v>0.78</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="11">
+        <v>8</v>
+      </c>
+      <c r="C25" s="14">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="D25" s="5">
+        <v>-4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="11">
+        <v>5</v>
+      </c>
+      <c r="C26" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="11">
+        <v>3</v>
+      </c>
+      <c r="C27" s="14">
+        <v>-0.51</v>
+      </c>
+      <c r="D27" s="5">
+        <v>-4.3E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="C28" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="D28" s="5">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="11">
+        <v>5</v>
+      </c>
+      <c r="C29" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="11">
+        <v>7</v>
+      </c>
+      <c r="C30" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="C31" s="14">
+        <v>-0.4</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="11">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14">
+        <v>-0.4</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="11">
+        <v>3</v>
+      </c>
+      <c r="C33" s="14">
+        <v>-0.44</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="C34" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="11">
+        <v>5</v>
+      </c>
+      <c r="C35" s="14">
+        <v>0.36</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="11">
+        <v>7</v>
+      </c>
+      <c r="C36" s="14">
+        <v>0.36</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="C37" s="14">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="D37" s="5">
+        <v>-5.5999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="11">
+        <v>5</v>
+      </c>
+      <c r="C38" s="14">
+        <v>-0.27</v>
+      </c>
+      <c r="D38" s="5">
+        <v>-1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="11">
+        <v>3</v>
+      </c>
+      <c r="C39" s="14">
+        <v>-0.27</v>
+      </c>
+      <c r="D39" s="5">
+        <v>-2.9899999999999998E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="C40" s="14">
+        <v>0.27</v>
+      </c>
+      <c r="D40" s="5">
+        <v>5.3000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="11">
+        <v>5</v>
+      </c>
+      <c r="C41" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="D41" s="5">
+        <v>6.6000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="11">
+        <v>5</v>
+      </c>
+      <c r="C42" s="14">
+        <v>0.27</v>
+      </c>
+      <c r="D42" s="5">
+        <v>6.6000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48" s="11"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="11"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="11"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="11"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="11"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="11"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="11"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B56" s="11"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B57" s="11"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B58" s="11"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B59" s="11"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B60" s="11"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B61" s="11"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B62" s="11"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="11"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B64" s="11"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="11"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="11"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="11"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="11"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="11"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="11"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>